<commit_message>
Update Optica BAC-10-Catálogo de conceptos.xlsx
</commit_message>
<xml_diff>
--- a/HT-4/Optica BAC-10-Catálogo de conceptos.xlsx
+++ b/HT-4/Optica BAC-10-Catálogo de conceptos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvill\Dropbox\uniandes\MATI\Notas de clase\Artefactos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E338E8E2-B2B7-435E-8FF1-26AE9626AB98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C07C5C5-4546-544A-BB72-DCE95EDB738D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
   <sheets>
     <sheet name="BAC-10" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Nombre</t>
   </si>
@@ -49,6 +49,78 @@
   </si>
   <si>
     <t>Definición</t>
+  </si>
+  <si>
+    <t>Óptica</t>
+  </si>
+  <si>
+    <t>Cliente</t>
+  </si>
+  <si>
+    <t>Montura</t>
+  </si>
+  <si>
+    <t>Lente</t>
+  </si>
+  <si>
+    <t>ProveedorLentes</t>
+  </si>
+  <si>
+    <t>ProveedorMonturas</t>
+  </si>
+  <si>
+    <t>Optómetra</t>
+  </si>
+  <si>
+    <t>Pago</t>
+  </si>
+  <si>
+    <t>Cotización</t>
+  </si>
+  <si>
+    <t>Factura</t>
+  </si>
+  <si>
+    <t>Fórmula</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un establecimiento en el que se venden monturas, se hacen lentes a la medida para las monturas, se reparan gafas y se hacen exámenes visuales </t>
+  </si>
+  <si>
+    <t>Persona compradora de los productos y servicios de la óptica</t>
+  </si>
+  <si>
+    <t>Estructura, generalmente de plástico o metal, que sostiene los lentes y reposa sobre la nariz y las orejas</t>
+  </si>
+  <si>
+    <t>Vidrio transparente utilizado para la corrección de la visión</t>
+  </si>
+  <si>
+    <t>Empresa a la que se le compran los lentes formulados o con modificaciones</t>
+  </si>
+  <si>
+    <t>Empresa a la que se le compran las monturas</t>
+  </si>
+  <si>
+    <t>Profesional de la salud especializado en el campo de la optometría</t>
+  </si>
+  <si>
+    <t>Concepto por el cual se retribuye una cierta cantidad de dinero a cambio de un bien o servicio recibido</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimado de cuánto cuesta una combinación de elementos que hacen un producto. En este caso, la fórmula, la montura, etc. </t>
+  </si>
+  <si>
+    <t>Documento que indica los productos pagados</t>
+  </si>
+  <si>
+    <t>Documento que indica el aumento necesario en cada ojo del paciente</t>
+  </si>
+  <si>
+    <t>Paciente</t>
+  </si>
+  <si>
+    <t>Persona que necesita un examen ocular para saber la corrección que debe tener en sus ojos</t>
   </si>
 </sst>
 </file>
@@ -121,11 +193,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -146,7 +220,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -444,107 +518,155 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="139" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.625" customWidth="1"/>
-    <col min="2" max="2" width="48.375" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
-      <c r="B15" s="5"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" s="5"/>
-      <c r="B16" s="5"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
-      <c r="B17" s="5"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.15">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.15">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.15">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="17" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.15">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.15">
+      <c r="A11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="30" x14ac:dyDescent="0.15">
+      <c r="A12" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="30" x14ac:dyDescent="0.15">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="45" x14ac:dyDescent="0.15">
+      <c r="A14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" x14ac:dyDescent="0.15">
+      <c r="A15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="30" x14ac:dyDescent="0.15">
+      <c r="A16" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.15">
+      <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A20" s="5"/>
       <c r="B20" s="5"/>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A21" s="5"/>
       <c r="B21" s="5"/>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A22" s="5"/>
       <c r="B22" s="5"/>
     </row>

</xml_diff>